<commit_message>
remove If nodes, fix bugs, remove word instructions
</commit_message>
<xml_diff>
--- a/template/Template_Excel_report.xlsx
+++ b/template/Template_Excel_report.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\CircularityTool4Revit\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B424CB4-DAC7-49F0-A6CA-4A1FF7AB09DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1373FF30-124F-4A27-A489-2BA575CAD8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{41215B07-995A-41B2-A990-0ED5E94562FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{41215B07-995A-41B2-A990-0ED5E94562FD}"/>
   </bookViews>
   <sheets>
     <sheet name="MCI_results" sheetId="5" r:id="rId1"/>
     <sheet name="PCI_results" sheetId="2" r:id="rId2"/>
-    <sheet name="Auxiliary" sheetId="6" r:id="rId3"/>
+    <sheet name="Auxiliary" sheetId="6" state="hidden" r:id="rId3"/>
     <sheet name="Report" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1188,7 +1188,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.59115824320906973</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.25</c:v>
@@ -1787,7 +1787,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.45978974471816531</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3717,8 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1913A91-03D4-487F-B764-AD4CEAA70EB7}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3823,7 +3823,7 @@
         <v>1234</v>
       </c>
       <c r="I2" s="11">
-        <v>0.4</v>
+        <v>800</v>
       </c>
       <c r="J2" s="11">
         <v>0.2</v>
@@ -3841,7 +3841,7 @@
         <v>0.2</v>
       </c>
       <c r="O2" s="11">
-        <v>0.4</v>
+        <v>500</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -3877,7 +3877,7 @@
         <v>288.435</v>
       </c>
       <c r="I3" s="11">
-        <v>0.6</v>
+        <v>100</v>
       </c>
       <c r="J3" s="11">
         <v>0.3</v>
@@ -3895,7 +3895,7 @@
         <v>0.3</v>
       </c>
       <c r="O3" s="11">
-        <v>0.6</v>
+        <v>200</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
@@ -4006,7 +4006,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4026,9 +4026,9 @@
         <f>MCI[[#Headers],[Virgin material (V)]]</f>
         <v>Virgin material (V)</v>
       </c>
-      <c r="C2" s="22">
-        <f>AVERAGE(MCI[Virgin material (V)])</f>
-        <v>0.5</v>
+      <c r="C2" s="26">
+        <f>AVERAGE(MCI[Virgin material (V)])/AVERAGE(MCI[Weight])</f>
+        <v>0.59115824320906973</v>
       </c>
       <c r="E2" s="21" t="str">
         <f>MCI[[#Headers],[For recycling (CR)]]</f>
@@ -4088,9 +4088,9 @@
         <f>MCI[[#Headers],[Linear waste (W0)]]</f>
         <v>Linear waste (W0)</v>
       </c>
-      <c r="F4" s="22">
-        <f>AVERAGE(MCI[Linear waste (W0)])</f>
-        <v>0.5</v>
+      <c r="F4" s="26">
+        <f>AVERAGE(MCI[Linear waste (W0)])/AVERAGE(MCI[Weight])</f>
+        <v>0.45978974471816531</v>
       </c>
       <c r="H4" s="21" t="str">
         <v>Plan Walls</v>
@@ -4232,8 +4232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6EEB95-C122-4F24-A6F8-574A63F65543}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -4494,8 +4494,8 @@
         <v>26</v>
       </c>
       <c r="E21" s="17">
-        <f>AVERAGE(MCI[Virgin material (V)])</f>
-        <v>0.5</v>
+        <f>AVERAGE(MCI[Virgin material (V)])/AVERAGE(MCI[Weight])</f>
+        <v>0.59115824320906973</v>
       </c>
       <c r="G21" s="33" t="s">
         <v>50</v>
@@ -4594,8 +4594,8 @@
         <v>34</v>
       </c>
       <c r="E27" s="17">
-        <f>AVERAGE(MCI[Linear waste (W0)])</f>
-        <v>0.5</v>
+        <f>AVERAGE(MCI[Linear waste (W0)])/AVERAGE(MCI[Weight])</f>
+        <v>0.45978974471816531</v>
       </c>
       <c r="P27" s="2"/>
     </row>

</xml_diff>

<commit_message>
add unknown to Excel
</commit_message>
<xml_diff>
--- a/template/Template_Excel_report.xlsx
+++ b/template/Template_Excel_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\CircularityTool4Revit\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB7F566-6768-4CD2-AA19-729BA45E32A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03DF9DB-7D3D-405B-AC91-6265CD8EB196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{41215B07-995A-41B2-A990-0ED5E94562FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{41215B07-995A-41B2-A990-0ED5E94562FD}"/>
   </bookViews>
   <sheets>
     <sheet name="MCI_results" sheetId="5" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Category</t>
   </si>
@@ -529,6 +529,9 @@
   </si>
   <si>
     <t>Average System Circularity Indicator</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,6 +653,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00BD7C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -700,7 +709,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -781,6 +790,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -830,10 +840,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFED00"/>
       <color rgb="FF00BD7C"/>
       <color rgb="FF444444"/>
       <color rgb="FFD123D1"/>
-      <color rgb="FFFFED00"/>
       <color rgb="FF66CCCC"/>
     </mruColors>
   </colors>
@@ -864,7 +874,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20511664440009586"/>
+          <c:y val="0.29061147132954024"/>
+          <c:w val="0.5811558028288093"/>
+          <c:h val="0.67408118086984548"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -963,6 +983,30 @@
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-4398-49DE-9473-8A41486B0AFB}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-65A2-4081-A915-7550540E5401}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1175,6 +1219,58 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="444444"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="nb-NO"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-65A2-4081-A915-7550540E5401}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1226,9 +1322,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Auxiliary!$B$2:$B$5</c:f>
+              <c:f>Auxiliary!$B$2:$B$6</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Virgin material (V)</c:v>
                 </c:pt>
@@ -1241,26 +1337,32 @@
                 <c:pt idx="3">
                   <c:v>Biological (FS)</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Unknown</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Auxiliary!$C$2:$C$5</c:f>
+              <c:f>Auxiliary!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.41666666666666663</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>0.42500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17499999999999999</c:v>
+                  <c:v>7.5000000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.05</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1292,6 +1394,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.0232126034327707E-2"/>
+          <c:y val="2.9962134467857549E-2"/>
+          <c:w val="0.97675654767695996"/>
+          <c:h val="0.17041140920332964"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1347,9 +1459,11 @@
     </a:p>
   </c:txPr>
   <c:printSettings>
-    <c:headerFooter/>
+    <c:headerFooter>
+      <c:oddHeader>&amp;L&amp;14&amp;K00BD7CCircularity Assessment&amp;C&amp;14&amp;K00BD7C&amp;D&amp;R&amp;G</c:oddHeader>
+    </c:headerFooter>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1586,7 +1700,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20797684679865558"/>
+          <c:y val="0.29636251890182369"/>
+          <c:w val="0.58404596284260246"/>
+          <c:h val="0.6680407493453131"/>
+        </c:manualLayout>
+      </c:layout>
       <c:pieChart>
         <c:varyColors val="1"/>
         <c:ser>
@@ -1661,6 +1785,32 @@
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-BEC5-4A04-A067-B00450F3C628}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-EA17-480F-ACA6-2645691C12AD}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1782,6 +1932,47 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="444444"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="nb-NO"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-EA17-480F-ACA6-2645691C12AD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1817,9 +2008,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Auxiliary!$E$2:$E$4</c:f>
+              <c:f>Auxiliary!$E$2:$E$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>For recycling (CR)</c:v>
                 </c:pt>
@@ -1829,23 +2020,29 @@
                 <c:pt idx="2">
                   <c:v>Linear waste (W0)</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>Unknown</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Auxiliary!$F$2:$F$4</c:f>
+              <c:f>Auxiliary!$F$2:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.27500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27500000000000002</c:v>
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1878,6 +2075,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.7674108521698725E-2"/>
+          <c:y val="2.9944261233420626E-2"/>
+          <c:w val="0.94901465249412598"/>
+          <c:h val="0.10605377077628729"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3474,7 +3681,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="EcoBIM">
+    <a:clrScheme name="Custom 1">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3500,7 +3707,7 @@
         <a:srgbClr val="00BD7C"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="EC1A92"/>
+        <a:srgbClr val="998E00"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="444444"/>
@@ -3770,33 +3977,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1913A91-03D4-487F-B764-AD4CEAA70EB7}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="1"/>
+    <col min="17" max="17" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75">
+    <row r="1" spans="1:17" ht="18">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3851,7 +4058,7 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1">
-        <v>12345678</v>
+        <v>9000123</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -3869,32 +4076,32 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>1200</v>
+        <v>2300</v>
       </c>
       <c r="H2" s="1">
         <f>MCI[[#This Row],[Volume]]*MCI[[#This Row],[Density]]</f>
-        <v>1200</v>
+        <v>2300</v>
       </c>
       <c r="I2" s="11">
-        <v>400</v>
+        <v>1725</v>
       </c>
       <c r="J2" s="11">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="K2" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="L2" s="11">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
         <v>0.15</v>
       </c>
-      <c r="L2" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="M2" s="11">
+      <c r="N2" s="11">
         <v>0.2</v>
       </c>
-      <c r="N2" s="11">
-        <v>0.3</v>
-      </c>
       <c r="O2" s="11">
-        <v>600</v>
+        <v>1495</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -3905,7 +4112,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1">
-        <v>1235465</v>
+        <v>9000124</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -3920,35 +4127,35 @@
         <v>49</v>
       </c>
       <c r="F3" s="8">
-        <v>0.123</v>
+        <v>0.5</v>
       </c>
       <c r="G3" s="1">
-        <v>2000</v>
+        <v>7850</v>
       </c>
       <c r="H3" s="1">
         <f>MCI[[#This Row],[Volume]]*MCI[[#This Row],[Density]]</f>
-        <v>246</v>
+        <v>3925</v>
       </c>
       <c r="I3" s="11">
-        <v>123</v>
+        <v>981.25</v>
       </c>
       <c r="J3" s="11">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
       <c r="K3" s="11">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="L3" s="11">
         <v>0</v>
       </c>
       <c r="M3" s="11">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="N3" s="11">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="O3" s="11">
-        <v>12.3</v>
+        <v>392.5</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
@@ -3975,14 +4182,14 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4059,15 +4266,15 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4081,7 +4288,7 @@
       </c>
       <c r="C2" s="24" cm="1">
         <f t="array" ref="C2">AVERAGE(MCI[Virgin material (V)]/MCI[Weight])</f>
-        <v>0.41666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="E2" s="19" t="str">
         <f>MCI[[#Headers],[For recycling (CR)]]</f>
@@ -4089,7 +4296,7 @@
       </c>
       <c r="F2" s="20">
         <f>AVERAGE(MCI[For recycling (CR)])</f>
-        <v>0.4</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>19</v>
@@ -4105,7 +4312,7 @@
       </c>
       <c r="C3" s="20">
         <f>AVERAGE(MCI[Recycled (FR)])</f>
-        <v>0.4</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="E3" s="19" t="str">
         <f>MCI[[#Headers],[For reuse (CU)]]</f>
@@ -4113,7 +4320,7 @@
       </c>
       <c r="F3" s="20">
         <f>AVERAGE(MCI[For reuse (CU)])</f>
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="H3" s="19" t="str" cm="1">
         <f t="array" ref="H3:H4">_xlfn.UNIQUE(PCI[Category])</f>
@@ -4135,7 +4342,7 @@
       </c>
       <c r="C4" s="20">
         <f>AVERAGE(MCI[Reused (FU)])</f>
-        <v>0.17499999999999999</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="E4" s="19" t="str">
         <f>MCI[[#Headers],[Linear waste (W0)]]</f>
@@ -4143,7 +4350,7 @@
       </c>
       <c r="F4" s="24" cm="1">
         <f t="array" ref="F4">AVERAGE(MCI[Linear waste (W0)]/MCI[Weight])</f>
-        <v>0.27500000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="H4" s="19" t="str">
         <v>Plan Walls</v>
@@ -4164,7 +4371,14 @@
       </c>
       <c r="C5" s="20">
         <f>AVERAGE(MCI[Biological (FS)])</f>
-        <v>0.05</v>
+        <v>0</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="36">
+        <f>IF(ABS(SUM(F2:F4)-1)&gt;0.01,ROUND(1-F2-F3-F4,3),0)</f>
+        <v>0</v>
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="23" t="str">
@@ -4177,6 +4391,13 @@
       </c>
     </row>
     <row r="6" spans="1:10">
+      <c r="B6" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="36">
+        <f>IF(ABS(SUM(C2:C5)-1)&gt;0.01,ROUND(1-C2-C3-C4-C5,3), 0)</f>
+        <v>0</v>
+      </c>
       <c r="H6" s="22"/>
       <c r="I6" s="23" t="str">
         <f>IF(ISBLANK(H6),"",AVERAGEIF(PCI[Category], Auxiliary!$H6, PCI[DisassemblyIndicator]))</f>
@@ -4285,178 +4506,178 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6EEB95-C122-4F24-A6F8-574A63F65543}">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="235" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="235" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" style="11" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="11" customWidth="1"/>
     <col min="6" max="6" width="2" customWidth="1"/>
-    <col min="7" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" customWidth="1"/>
+    <col min="7" max="13" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.899999999999999" customHeight="1">
+    <row r="1" spans="1:16" ht="16.95" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="G1" s="41" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="G1" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41" t="s">
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="16.7" customHeight="1">
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="16.649999999999999" customHeight="1">
       <c r="A2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="16.7" customHeight="1">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="16.649999999999999" customHeight="1">
       <c r="A3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="11.25" customHeight="1">
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="8.4" customHeight="1">
       <c r="C4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:16" ht="19.899999999999999" customHeight="1">
-      <c r="A5" s="46" t="s">
+    <row r="5" spans="1:16" ht="19.95" customHeight="1">
+      <c r="A5" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="19.899999999999999" customHeight="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
+    <row r="6" spans="1:16" ht="19.95" customHeight="1">
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" s="11" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+    <row r="7" spans="1:16" s="11" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="1:16" s="11" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
+    <row r="8" spans="1:16" s="11" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" spans="1:16" s="11" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+    <row r="9" spans="1:16" s="11" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:16" ht="19.899999999999999" customHeight="1">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+    <row r="11" spans="1:16" ht="19.95" customHeight="1">
+      <c r="A11" s="47"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="19.899999999999999" customHeight="1">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+    <row r="12" spans="1:16" ht="19.95" customHeight="1">
+      <c r="A12" s="47"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="19.899999999999999" customHeight="1">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="40"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
       <c r="P13" s="13"/>
     </row>
-    <row r="14" spans="1:16" ht="11.25" customHeight="1">
+    <row r="14" spans="1:16" ht="9" customHeight="1">
       <c r="A14" s="1"/>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A15" s="44" t="s">
+    <row r="15" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A15" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="9" t="s">
         <v>16</v>
       </c>
@@ -4465,12 +4686,12 @@
       </c>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A16" s="44" t="s">
+    <row r="16" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A16" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="9" t="s">
         <v>17</v>
       </c>
@@ -4479,12 +4700,12 @@
       </c>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A17" s="44" t="s">
+    <row r="17" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A17" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="29" t="s">
         <v>18</v>
       </c>
@@ -4494,14 +4715,14 @@
       </c>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A18" s="37" t="s">
+    <row r="18" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A18" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="43"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="7" t="s">
         <v>19</v>
       </c>
@@ -4511,12 +4732,12 @@
       </c>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A19" s="38"/>
-      <c r="B19" s="44" t="s">
+    <row r="19" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A19" s="39"/>
+      <c r="B19" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="44"/>
+      <c r="C19" s="45"/>
       <c r="D19" s="7" t="s">
         <v>21</v>
       </c>
@@ -4526,12 +4747,12 @@
       </c>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A20" s="39"/>
-      <c r="B20" s="42" t="s">
+    <row r="20" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A20" s="40"/>
+      <c r="B20" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="42"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="29" t="s">
         <v>22</v>
       </c>
@@ -4541,140 +4762,140 @@
       </c>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:16" s="14" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A21" s="37" t="s">
+    <row r="21" spans="1:16" s="14" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A21" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="43"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="34" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="35" cm="1">
         <f t="array" ref="E21">AVERAGE(MCI[Virgin material (V)]/MCI[Weight])</f>
-        <v>0.41666666666666663</v>
-      </c>
-      <c r="G21" s="45" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
       <c r="P21" s="15"/>
     </row>
-    <row r="22" spans="1:16" s="14" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A22" s="38"/>
-      <c r="B22" s="36" t="s">
+    <row r="22" spans="1:16" s="14" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A22" s="39"/>
+      <c r="B22" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="36"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="32" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="33">
         <f>AVERAGE(MCI[Recycled (FR)])</f>
-        <v>0.4</v>
+        <v>0.42500000000000004</v>
       </c>
       <c r="P22" s="15"/>
     </row>
-    <row r="23" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A23" s="38"/>
-      <c r="B23" s="36" t="s">
+    <row r="23" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A23" s="39"/>
+      <c r="B23" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="32" t="s">
         <v>24</v>
       </c>
       <c r="E23" s="33">
         <f>AVERAGE(MCI[Reused (FU)])</f>
-        <v>0.17499999999999999</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="P23" s="5"/>
     </row>
-    <row r="24" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="42" t="s">
+    <row r="24" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A24" s="40"/>
+      <c r="B24" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="42"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="29" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="30">
         <f>AVERAGE(MCI[Biological (FS)])</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="1:16" s="4" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A25" s="38" t="s">
+    <row r="25" spans="1:16" s="4" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A25" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="36"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="32" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="33">
         <f>AVERAGE(MCI[For recycling (CR)])</f>
-        <v>0.4</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="1:16" ht="19.899999999999999" customHeight="1">
-      <c r="A26" s="38"/>
-      <c r="B26" s="36" t="s">
+    <row r="26" spans="1:16" ht="19.95" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="36"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="32" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="33">
         <f>AVERAGE(MCI[For reuse (CU)])</f>
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" ht="19.899999999999999" customHeight="1">
-      <c r="A27" s="38"/>
-      <c r="B27" s="36" t="s">
+    <row r="27" spans="1:16" ht="19.95" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="36"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="32" t="s">
         <v>28</v>
       </c>
       <c r="E27" s="33" cm="1">
         <f t="array" ref="E27">AVERAGE(MCI[Linear waste (W0)]/MCI[Weight])</f>
-        <v>0.27500000000000002</v>
+        <v>0.375</v>
       </c>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" ht="19.899999999999999" customHeight="1"/>
-    <row r="29" spans="1:16" ht="19.899999999999999" customHeight="1">
+    <row r="28" spans="1:16" ht="19.95" customHeight="1"/>
+    <row r="29" spans="1:16" ht="19.95" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:16" ht="19.899999999999999" customHeight="1"/>
-    <row r="31" spans="1:16" ht="19.899999999999999" customHeight="1"/>
-    <row r="32" spans="1:16" ht="19.899999999999999" customHeight="1"/>
-    <row r="33" ht="19.899999999999999" customHeight="1"/>
-    <row r="34" ht="19.899999999999999" customHeight="1"/>
-    <row r="35" ht="19.899999999999999" customHeight="1"/>
-    <row r="36" ht="19.899999999999999" customHeight="1"/>
+    <row r="30" spans="1:16" ht="19.95" customHeight="1"/>
+    <row r="31" spans="1:16" ht="19.95" customHeight="1"/>
+    <row r="32" spans="1:16" ht="19.95" customHeight="1"/>
+    <row r="33" ht="19.95" customHeight="1"/>
+    <row r="34" ht="19.95" customHeight="1"/>
+    <row r="35" ht="19.95" customHeight="1"/>
+    <row r="36" ht="19.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="25">
     <mergeCell ref="K1:N1"/>
@@ -4703,7 +4924,7 @@
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B21:C21"/>
   </mergeCells>
-  <pageMargins left="0.57189542483660127" right="0.71794871794871795" top="0.60457516339869277" bottom="0.54738562091503273" header="0.3" footer="0.3"/>
+  <pageMargins left="0.57189542483660127" right="0.71794871794871795" top="0.60457516339869277" bottom="0.39583333333333331" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;14&amp;K00BD7CCircularity Assessment&amp;C&amp;14&amp;K00BD7C&amp;D&amp;R&amp;G</oddHeader>

</xml_diff>